<commit_message>
delete duplicate file, and switch to log10 errors
</commit_message>
<xml_diff>
--- a/Examples/BoundedProductivity/Results/Results.xlsx
+++ b/Examples/BoundedProductivity/Results/Results.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14175" windowHeight="8985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14175" windowHeight="8985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="39">
   <si>
     <t>Seconds</t>
   </si>
@@ -99,12 +101,57 @@
   </si>
   <si>
     <t>order3nocubature140.mat</t>
+  </si>
+  <si>
+    <t>Bound In Model</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Cubature</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Monomial, Degree 3</t>
+  </si>
+  <si>
+    <t>Sparse, Degree 3</t>
+  </si>
+  <si>
+    <t>Sparse, Degree 5</t>
+  </si>
+  <si>
+    <t>Sparse, Degree 7</t>
+  </si>
+  <si>
+    <t>QMC, 15 Points</t>
+  </si>
+  <si>
+    <t>QMC, 31 Points</t>
+  </si>
+  <si>
+    <t>QMC, 63 Points</t>
+  </si>
+  <si>
+    <t>QMC, 1023 Points</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,8 +181,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -229,6 +279,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -264,6 +331,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -418,11 +502,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -920,4 +1007,1312 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="A1:Q11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>65.924000000000007</v>
+      </c>
+      <c r="C5" s="1">
+        <v>62.12</v>
+      </c>
+      <c r="D5" s="1">
+        <v>53.027999999999999</v>
+      </c>
+      <c r="E5" s="1">
+        <v>141.298</v>
+      </c>
+      <c r="F5" s="1">
+        <v>138.892</v>
+      </c>
+      <c r="G5" s="1">
+        <v>139.83099999999999</v>
+      </c>
+      <c r="H5" s="1">
+        <v>274.37400000000002</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1537.27</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1397.2919999999999</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1794.4839999999999</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1840.154</v>
+      </c>
+      <c r="M5" s="1">
+        <v>2009.1079999999999</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1965.1559999999999</v>
+      </c>
+      <c r="O5" s="1">
+        <v>2214.1790000000001</v>
+      </c>
+      <c r="P5" s="1">
+        <v>3183.7289999999998</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>5197.2809999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>6.1250000000000443E-4</v>
+      </c>
+      <c r="C6">
+        <v>1.5234992087331811E-17</v>
+      </c>
+      <c r="D6">
+        <v>1.9924383323766116E-17</v>
+      </c>
+      <c r="E6">
+        <v>3.6697402541254545E-3</v>
+      </c>
+      <c r="F6">
+        <v>3.7623246035838344E-3</v>
+      </c>
+      <c r="G6">
+        <v>3.7623246035838535E-3</v>
+      </c>
+      <c r="H6">
+        <v>7.3157992741799916E-4</v>
+      </c>
+      <c r="I6">
+        <v>4.1837520523788454E-4</v>
+      </c>
+      <c r="J6">
+        <v>4.1837520523789674E-4</v>
+      </c>
+      <c r="K6">
+        <v>9.6459132732167432E-4</v>
+      </c>
+      <c r="L6">
+        <v>9.6459132732167432E-4</v>
+      </c>
+      <c r="M6">
+        <v>5.2466878968746922E-4</v>
+      </c>
+      <c r="N6">
+        <v>9.1245070107061018E-4</v>
+      </c>
+      <c r="O6">
+        <v>5.9750361728672444E-4</v>
+      </c>
+      <c r="P6">
+        <v>4.0391347234567564E-4</v>
+      </c>
+      <c r="Q6">
+        <v>1.5691691209492945E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>6.1250000000000215E-4</v>
+      </c>
+      <c r="C7">
+        <v>2.3553479593040681E-17</v>
+      </c>
+      <c r="D7">
+        <v>2.7185765752604614E-17</v>
+      </c>
+      <c r="E7">
+        <v>6.0511199503417643E-3</v>
+      </c>
+      <c r="F7">
+        <v>6.3913804489182258E-3</v>
+      </c>
+      <c r="G7">
+        <v>6.3913804489182354E-3</v>
+      </c>
+      <c r="H7">
+        <v>8.4527059632430067E-4</v>
+      </c>
+      <c r="I7">
+        <v>6.7270190385518682E-4</v>
+      </c>
+      <c r="J7">
+        <v>6.727019038551918E-4</v>
+      </c>
+      <c r="K7">
+        <v>1.6715978163539646E-3</v>
+      </c>
+      <c r="L7">
+        <v>1.6715978163539646E-3</v>
+      </c>
+      <c r="M7">
+        <v>9.2986664864833416E-4</v>
+      </c>
+      <c r="N7">
+        <v>1.2721420015818616E-3</v>
+      </c>
+      <c r="O7">
+        <v>8.171980111514914E-4</v>
+      </c>
+      <c r="P7">
+        <v>5.4891737098515644E-4</v>
+      </c>
+      <c r="Q7">
+        <v>2.3018054918998011E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>6.1250000000012683E-4</v>
+      </c>
+      <c r="C8">
+        <v>1.6653345369377348E-16</v>
+      </c>
+      <c r="D8">
+        <v>1.1102230246251565E-16</v>
+      </c>
+      <c r="E8">
+        <v>1.3131704259106237E-2</v>
+      </c>
+      <c r="F8">
+        <v>1.3744204259106253E-2</v>
+      </c>
+      <c r="G8">
+        <v>1.3744204259106281E-2</v>
+      </c>
+      <c r="H8">
+        <v>1.8831645103120284E-3</v>
+      </c>
+      <c r="I8">
+        <v>1.9660006775838595E-3</v>
+      </c>
+      <c r="J8">
+        <v>1.9660006775839844E-3</v>
+      </c>
+      <c r="K8">
+        <v>3.8489078816211428E-3</v>
+      </c>
+      <c r="L8">
+        <v>3.8489078816211428E-3</v>
+      </c>
+      <c r="M8">
+        <v>2.1735009363887184E-3</v>
+      </c>
+      <c r="N8">
+        <v>2.1689279739632375E-3</v>
+      </c>
+      <c r="O8">
+        <v>1.393415715757497E-3</v>
+      </c>
+      <c r="P8">
+        <v>9.5470159249545078E-4</v>
+      </c>
+      <c r="Q8">
+        <v>4.4527440716839867E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>1.3131704259106125E-2</v>
+      </c>
+      <c r="F9">
+        <v>1.3744204259106109E-2</v>
+      </c>
+      <c r="G9">
+        <v>1.3744204259106125E-2</v>
+      </c>
+      <c r="H9">
+        <v>7.4031924046243113E-4</v>
+      </c>
+      <c r="I9">
+        <v>1.2781924046242373E-4</v>
+      </c>
+      <c r="J9">
+        <v>1.2781924046241378E-4</v>
+      </c>
+      <c r="K9">
+        <v>3.8489078816210053E-3</v>
+      </c>
+      <c r="L9">
+        <v>3.8489078816210053E-3</v>
+      </c>
+      <c r="M9">
+        <v>2.1735009363885718E-3</v>
+      </c>
+      <c r="N9">
+        <v>2.1689279739630831E-3</v>
+      </c>
+      <c r="O9">
+        <v>1.3934157157573625E-3</v>
+      </c>
+      <c r="P9">
+        <v>9.5470159249529888E-4</v>
+      </c>
+      <c r="Q9">
+        <v>4.452744071682562E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>1.3131704259106116E-2</v>
+      </c>
+      <c r="F10">
+        <v>1.374420425910612E-2</v>
+      </c>
+      <c r="G10">
+        <v>1.3744204259106132E-2</v>
+      </c>
+      <c r="H10">
+        <v>7.4031924046243016E-4</v>
+      </c>
+      <c r="I10">
+        <v>1.2781924046242378E-4</v>
+      </c>
+      <c r="J10">
+        <v>1.2781924046241378E-4</v>
+      </c>
+      <c r="K10">
+        <v>3.8489078816210031E-3</v>
+      </c>
+      <c r="L10">
+        <v>3.8489078816210031E-3</v>
+      </c>
+      <c r="M10">
+        <v>2.1735009363885696E-3</v>
+      </c>
+      <c r="N10">
+        <v>2.1689279739630814E-3</v>
+      </c>
+      <c r="O10">
+        <v>1.3934157157573638E-3</v>
+      </c>
+      <c r="P10">
+        <v>9.547015924953004E-4</v>
+      </c>
+      <c r="Q10">
+        <v>4.4527440716825685E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>1.3131704259106237E-2</v>
+      </c>
+      <c r="F11">
+        <v>1.3744204259106253E-2</v>
+      </c>
+      <c r="G11">
+        <v>1.3744204259106281E-2</v>
+      </c>
+      <c r="H11">
+        <v>7.4031924046261133E-4</v>
+      </c>
+      <c r="I11">
+        <v>1.2781924046262327E-4</v>
+      </c>
+      <c r="J11">
+        <v>1.2781924046259552E-4</v>
+      </c>
+      <c r="K11">
+        <v>3.8489078816211428E-3</v>
+      </c>
+      <c r="L11">
+        <v>3.8489078816211428E-3</v>
+      </c>
+      <c r="M11">
+        <v>2.1735009363887184E-3</v>
+      </c>
+      <c r="N11">
+        <v>2.1689279739632375E-3</v>
+      </c>
+      <c r="O11">
+        <v>1.393415715757497E-3</v>
+      </c>
+      <c r="P11">
+        <v>9.5470159249545078E-4</v>
+      </c>
+      <c r="Q11">
+        <v>4.4527440716839867E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState columnSort="1" ref="B1:Q13">
+    <sortCondition ref="B5:Q5"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1">
+        <f>VLOOKUP(Sheet3!$A3,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>65.924000000000007</v>
+      </c>
+      <c r="F3" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A3,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-3.2128939069634268</v>
+      </c>
+      <c r="G3" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A3,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-3.2128939069634286</v>
+      </c>
+      <c r="H3" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A3,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-3.2128939069633402</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="1">
+        <f>VLOOKUP(Sheet3!$A4,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>62.12</v>
+      </c>
+      <c r="F4" s="2">
+        <f>LOG10(VLOOKUP(Sheet3!$A4,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-16.817157767002779</v>
+      </c>
+      <c r="G4" s="2">
+        <f>LOG10(VLOOKUP(Sheet3!$A4,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-16.627944924780191</v>
+      </c>
+      <c r="H4" s="2">
+        <f>LOG10(VLOOKUP(Sheet3!$A4,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-15.778498511135322</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1">
+        <f>VLOOKUP(Sheet3!$A5,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>53.027999999999999</v>
+      </c>
+      <c r="F5" s="2">
+        <f>LOG10(VLOOKUP(Sheet3!$A5,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-16.700615111499232</v>
+      </c>
+      <c r="G5" s="2">
+        <f>LOG10(VLOOKUP(Sheet3!$A5,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-16.565658429539337</v>
+      </c>
+      <c r="H5" s="2">
+        <f>LOG10(VLOOKUP(Sheet3!$A5,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-15.954589770191003</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1">
+        <f>VLOOKUP(Sheet3!$A6,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>141.298</v>
+      </c>
+      <c r="F6" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A6,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-2.4353646742198873</v>
+      </c>
+      <c r="G6" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A6,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-2.218164238035147</v>
+      </c>
+      <c r="H6" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A6,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-1.8816789066375281</v>
+      </c>
+      <c r="I6" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A6,Sheet1!$A$2:$I$17,I$2,FALSE))</f>
+        <v>-1.8816789066375319</v>
+      </c>
+      <c r="J6" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A6,Sheet1!$A$2:$I$17,J$2,FALSE))</f>
+        <v>-1.8816789066375321</v>
+      </c>
+      <c r="K6" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A6,Sheet1!$A$2:$I$17,K$2,FALSE))</f>
+        <v>-1.8816789066375281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1">
+        <f>VLOOKUP(Sheet3!$A7,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>138.892</v>
+      </c>
+      <c r="F7" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A7,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-2.4245437373705219</v>
+      </c>
+      <c r="G7" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A7,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-2.1944053301672723</v>
+      </c>
+      <c r="H7" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A7,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-1.861880399209606</v>
+      </c>
+      <c r="I7" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A7,Sheet1!$A$2:$I$17,I$2,FALSE))</f>
+        <v>-1.8618803992096105</v>
+      </c>
+      <c r="J7" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A7,Sheet1!$A$2:$I$17,J$2,FALSE))</f>
+        <v>-1.8618803992096102</v>
+      </c>
+      <c r="K7" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A7,Sheet1!$A$2:$I$17,K$2,FALSE))</f>
+        <v>-1.861880399209606</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1">
+        <f>VLOOKUP(Sheet3!$A8,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>139.83099999999999</v>
+      </c>
+      <c r="F8" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A8,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-2.4245437373705196</v>
+      </c>
+      <c r="G8" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A8,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-2.1944053301672715</v>
+      </c>
+      <c r="H8" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A8,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-1.8618803992096051</v>
+      </c>
+      <c r="I8" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A8,Sheet1!$A$2:$I$17,I$2,FALSE))</f>
+        <v>-1.86188039920961</v>
+      </c>
+      <c r="J8" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A8,Sheet1!$A$2:$I$17,J$2,FALSE))</f>
+        <v>-1.8618803992096098</v>
+      </c>
+      <c r="K8" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A8,Sheet1!$A$2:$I$17,K$2,FALSE))</f>
+        <v>-1.8618803992096051</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="1">
+        <f>VLOOKUP(Sheet3!$A9,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>274.37400000000002</v>
+      </c>
+      <c r="F9" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A9,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-3.1357382189025516</v>
+      </c>
+      <c r="G9" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A9,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-3.0730042381770852</v>
+      </c>
+      <c r="H9" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A9,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-2.7251117390380686</v>
+      </c>
+      <c r="I9" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A9,Sheet1!$A$2:$I$17,I$2,FALSE))</f>
+        <v>-3.1305809634125055</v>
+      </c>
+      <c r="J9" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A9,Sheet1!$A$2:$I$17,J$2,FALSE))</f>
+        <v>-3.1305809634125064</v>
+      </c>
+      <c r="K9" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A9,Sheet1!$A$2:$I$17,K$2,FALSE))</f>
+        <v>-3.1305809634123998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1">
+        <f>VLOOKUP(Sheet3!$A10,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>1537.27</v>
+      </c>
+      <c r="F10" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A10,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-3.3784340615868791</v>
+      </c>
+      <c r="G10" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A10,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-3.1721773431918345</v>
+      </c>
+      <c r="H10" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A10,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-2.7064163368238829</v>
+      </c>
+      <c r="I10" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A10,Sheet1!$A$2:$I$17,I$2,FALSE))</f>
+        <v>-3.8934037674787341</v>
+      </c>
+      <c r="J10" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A10,Sheet1!$A$2:$I$17,J$2,FALSE))</f>
+        <v>-3.8934037674787336</v>
+      </c>
+      <c r="K10" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A10,Sheet1!$A$2:$I$17,K$2,FALSE))</f>
+        <v>-3.8934037674780559</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1">
+        <f>VLOOKUP(Sheet3!$A11,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>1397.2919999999999</v>
+      </c>
+      <c r="F11" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A11,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-3.3784340615868662</v>
+      </c>
+      <c r="G11" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A11,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-3.1721773431918314</v>
+      </c>
+      <c r="H11" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A11,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-2.7064163368238554</v>
+      </c>
+      <c r="I11" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A11,Sheet1!$A$2:$I$17,I$2,FALSE))</f>
+        <v>-3.8934037674787678</v>
+      </c>
+      <c r="J11" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A11,Sheet1!$A$2:$I$17,J$2,FALSE))</f>
+        <v>-3.8934037674787678</v>
+      </c>
+      <c r="K11" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A11,Sheet1!$A$2:$I$17,K$2,FALSE))</f>
+        <v>-3.8934037674781501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1">
+        <f>VLOOKUP(Sheet3!$A12,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>1794.4839999999999</v>
+      </c>
+      <c r="F12" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A12,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-3.015656647155244</v>
+      </c>
+      <c r="G12" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A12,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-2.7768682048567457</v>
+      </c>
+      <c r="H12" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A12,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-2.4146624830291725</v>
+      </c>
+      <c r="I12" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A12,Sheet1!$A$2:$I$17,I$2,FALSE))</f>
+        <v>-2.4146624830291881</v>
+      </c>
+      <c r="J12" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A12,Sheet1!$A$2:$I$17,J$2,FALSE))</f>
+        <v>-2.4146624830291885</v>
+      </c>
+      <c r="K12" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A12,Sheet1!$A$2:$I$17,K$2,FALSE))</f>
+        <v>-2.4146624830291725</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="1">
+        <f>VLOOKUP(Sheet3!$A13,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>1840.154</v>
+      </c>
+      <c r="F13" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A13,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-3.015656647155244</v>
+      </c>
+      <c r="G13" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A13,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-2.7768682048567457</v>
+      </c>
+      <c r="H13" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A13,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-2.4146624830291725</v>
+      </c>
+      <c r="I13" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A13,Sheet1!$A$2:$I$17,I$2,FALSE))</f>
+        <v>-2.4146624830291881</v>
+      </c>
+      <c r="J13" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A13,Sheet1!$A$2:$I$17,J$2,FALSE))</f>
+        <v>-2.4146624830291885</v>
+      </c>
+      <c r="K13" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A13,Sheet1!$A$2:$I$17,K$2,FALSE))</f>
+        <v>-2.4146624830291725</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="1">
+        <f>VLOOKUP(Sheet3!$A14,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>2009.1079999999999</v>
+      </c>
+      <c r="F14" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A14,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-3.2801147693630321</v>
+      </c>
+      <c r="G14" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A14,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-3.0315793287672097</v>
+      </c>
+      <c r="H14" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A14,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-2.6628401683701464</v>
+      </c>
+      <c r="I14" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A14,Sheet1!$A$2:$I$17,I$2,FALSE))</f>
+        <v>-2.6628401683701757</v>
+      </c>
+      <c r="J14" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A14,Sheet1!$A$2:$I$17,J$2,FALSE))</f>
+        <v>-2.6628401683701761</v>
+      </c>
+      <c r="K14" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A14,Sheet1!$A$2:$I$17,K$2,FALSE))</f>
+        <v>-2.6628401683701464</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="1">
+        <f>VLOOKUP(Sheet3!$A15,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>1965.1559999999999</v>
+      </c>
+      <c r="F15" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A15,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-3.0397905907962834</v>
+      </c>
+      <c r="G15" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A15,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-2.8954644082934684</v>
+      </c>
+      <c r="H15" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A15,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-2.663754869852887</v>
+      </c>
+      <c r="I15" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A15,Sheet1!$A$2:$I$17,I$2,FALSE))</f>
+        <v>-2.6637548698529181</v>
+      </c>
+      <c r="J15" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A15,Sheet1!$A$2:$I$17,J$2,FALSE))</f>
+        <v>-2.6637548698529181</v>
+      </c>
+      <c r="K15" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A15,Sheet1!$A$2:$I$17,K$2,FALSE))</f>
+        <v>-2.663754869852887</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="1">
+        <f>VLOOKUP(Sheet3!$A16,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>2214.1790000000001</v>
+      </c>
+      <c r="F16" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A16,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-3.2236594611531997</v>
+      </c>
+      <c r="G16" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A16,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-3.0876726989986989</v>
+      </c>
+      <c r="H16" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A16,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-2.8559192955466268</v>
+      </c>
+      <c r="I16" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A16,Sheet1!$A$2:$I$17,I$2,FALSE))</f>
+        <v>-2.8559192955466686</v>
+      </c>
+      <c r="J16" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A16,Sheet1!$A$2:$I$17,J$2,FALSE))</f>
+        <v>-2.8559192955466681</v>
+      </c>
+      <c r="K16" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A16,Sheet1!$A$2:$I$17,K$2,FALSE))</f>
+        <v>-2.8559192955466268</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="1">
+        <f>VLOOKUP(Sheet3!$A17,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>3183.7289999999998</v>
+      </c>
+      <c r="F17" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A17,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-3.3937116608983304</v>
+      </c>
+      <c r="G17" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A17,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-3.2604930253604381</v>
+      </c>
+      <c r="H17" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A17,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-3.0201323530070989</v>
+      </c>
+      <c r="I17" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A17,Sheet1!$A$2:$I$17,I$2,FALSE))</f>
+        <v>-3.0201323530071682</v>
+      </c>
+      <c r="J17" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A17,Sheet1!$A$2:$I$17,J$2,FALSE))</f>
+        <v>-3.0201323530071673</v>
+      </c>
+      <c r="K17" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A17,Sheet1!$A$2:$I$17,K$2,FALSE))</f>
+        <v>-3.0201323530070989</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="1">
+        <f>VLOOKUP(Sheet3!$A18,Sheet1!$A$2:$I$17,E$2,FALSE)</f>
+        <v>5197.2809999999999</v>
+      </c>
+      <c r="F18" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A18,Sheet1!$A$2:$I$17,F$2,FALSE))</f>
+        <v>-3.8043302467655948</v>
+      </c>
+      <c r="G18" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A18,Sheet1!$A$2:$I$17,G$2,FALSE))</f>
+        <v>-3.6379313780839944</v>
+      </c>
+      <c r="H18" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A18,Sheet1!$A$2:$I$17,H$2,FALSE))</f>
+        <v>-3.3513722658949514</v>
+      </c>
+      <c r="I18" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A18,Sheet1!$A$2:$I$17,I$2,FALSE))</f>
+        <v>-3.3513722658950904</v>
+      </c>
+      <c r="J18" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A18,Sheet1!$A$2:$I$17,J$2,FALSE))</f>
+        <v>-3.35137226589509</v>
+      </c>
+      <c r="K18" s="3">
+        <f>LOG10(VLOOKUP(Sheet3!$A18,Sheet1!$A$2:$I$17,K$2,FALSE))</f>
+        <v>-3.3513722658949514</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>